<commit_message>
Corrected optimizer logic. Added pop up when Optimizer run is made. Removed hard coded values with session values in key areas
</commit_message>
<xml_diff>
--- a/data/Data Request Detailed_23062025.xlsx
+++ b/data/Data Request Detailed_23062025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Anshul_Agarwal/Library/CloudStorage/Box-Box/DCM/99 Working folders/14 Anshul/Margin Maximizer/integrated_margin_maximizer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B7A523-3D96-E043-81DB-44B65B80F160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA77B06-FDA7-F04D-973F-FD68F33DF368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="860" windowWidth="21160" windowHeight="14300" activeTab="3" xr2:uid="{B49C1CC5-7DB3-794A-B170-F3399E5F60B1}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="30000" windowHeight="16580" activeTab="3" xr2:uid="{B49C1CC5-7DB3-794A-B170-F3399E5F60B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Request" sheetId="1" state="hidden" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1717" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1718" uniqueCount="459">
   <si>
     <t>Type</t>
   </si>
@@ -6113,18 +6113,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A30"/>
+    <mergeCell ref="B2:B30"/>
+    <mergeCell ref="B31:B51"/>
+    <mergeCell ref="A31:A51"/>
+    <mergeCell ref="A52:A75"/>
+    <mergeCell ref="B52:B75"/>
     <mergeCell ref="A76:A86"/>
     <mergeCell ref="B76:B86"/>
     <mergeCell ref="A87:A97"/>
     <mergeCell ref="B87:B97"/>
     <mergeCell ref="A98:A110"/>
     <mergeCell ref="B98:B110"/>
-    <mergeCell ref="A2:A30"/>
-    <mergeCell ref="B2:B30"/>
-    <mergeCell ref="B31:B51"/>
-    <mergeCell ref="A31:A51"/>
-    <mergeCell ref="A52:A75"/>
-    <mergeCell ref="B52:B75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -11314,8 +11314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC5ED671-0947-D741-A9ED-72DD6B28D57E}">
   <dimension ref="A1:Q138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K120" workbookViewId="0">
-      <selection activeCell="S134" sqref="S134"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="140" workbookViewId="0">
+      <selection activeCell="O46" sqref="O46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12758,6 +12758,9 @@
       </c>
       <c r="N45" t="s">
         <v>218</v>
+      </c>
+      <c r="O45" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>